<commit_message>
Modification de la roadmap
</commit_message>
<xml_diff>
--- a/textes/Roadmap.xlsx
+++ b/textes/Roadmap.xlsx
@@ -2775,15 +2775,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1485900</xdr:colOff>
+      <xdr:colOff>1485899</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4025900</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
+      <xdr:rowOff>206375</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2798,8 +2798,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5448300" y="3429000"/>
-          <a:ext cx="2540000" cy="203200"/>
+          <a:off x="5454649" y="3429000"/>
+          <a:ext cx="6769101" cy="174625"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2852,11 +2852,11 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>1460500</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4000500</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
@@ -2873,8 +2873,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5422900" y="3670300"/>
-          <a:ext cx="2540000" cy="215900"/>
+          <a:off x="5429250" y="3683000"/>
+          <a:ext cx="6778625" cy="184150"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2915,7 +2915,27 @@
               <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>MEP Profil, Paramètres, Contact</a:t>
+            <a:t>MEP Modification</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> de profil, Paramètresz de profil, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Contact</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2930,10 +2950,10 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4038600</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>241300</xdr:rowOff>
+      <xdr:rowOff>222250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2948,8 +2968,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4025900" y="3937000"/>
-          <a:ext cx="3975100" cy="228600"/>
+          <a:off x="4032250" y="3917950"/>
+          <a:ext cx="8159750" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3000,7 +3020,7 @@
               <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> voyages, Détails voyage</a:t>
+            <a:t> voyages, Détails voyage, Mes amis</a:t>
           </a:r>
           <a:endParaRPr lang="en-IN" sz="1100">
             <a:solidFill>
@@ -3017,15 +3037,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>50799</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>12699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4038600</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:rowOff>238124</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3040,8 +3060,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4013200" y="4191000"/>
-          <a:ext cx="3987800" cy="215900"/>
+          <a:off x="4019549" y="4171949"/>
+          <a:ext cx="8235951" cy="225425"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3092,7 +3112,7 @@
               <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> voyage, Messages privés</a:t>
+            <a:t> voyage, Profil</a:t>
           </a:r>
           <a:endParaRPr lang="en-IN" sz="1100">
             <a:solidFill>
@@ -3186,13 +3206,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:rowOff>247649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4064000</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:rowOff>238124</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3207,8 +3227,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5492750" y="2136775"/>
-          <a:ext cx="2540000" cy="203200"/>
+          <a:off x="5492750" y="2136774"/>
+          <a:ext cx="6667500" cy="244475"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3261,13 +3281,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
+      <xdr:rowOff>22224</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4032250</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>212725</xdr:rowOff>
+      <xdr:rowOff>222249</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3282,8 +3302,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4064000" y="2419350"/>
-          <a:ext cx="3937000" cy="190500"/>
+          <a:off x="4064000" y="2419349"/>
+          <a:ext cx="8096250" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3336,13 +3356,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>79375</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>25399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4016375</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>15874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3357,8 +3377,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4048125" y="2676525"/>
-          <a:ext cx="3937000" cy="190500"/>
+          <a:off x="4048125" y="2676524"/>
+          <a:ext cx="8128000" cy="244475"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3411,13 +3431,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>79375</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>25399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4016375</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
+      <xdr:rowOff>238124</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3432,8 +3452,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4048125" y="2930525"/>
-          <a:ext cx="3937000" cy="190500"/>
+          <a:off x="4048125" y="2930524"/>
+          <a:ext cx="8191500" cy="212725"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -8658,7 +8678,7 @@
   <dimension ref="B1:N35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>